<commit_message>
Alteração lista de requisitos
</commit_message>
<xml_diff>
--- a/Documentacao/Sprint1/DocumentacaoPrevia/ListaRequisitos.xlsx
+++ b/Documentacao/Sprint1/DocumentacaoPrevia/ListaRequisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\PI\SM ULTIMATE\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOLE201901\Desktop\PiOrion\OrionConecta\Documentacao\Sprint1\DocumentacaoPrevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E9E35-E75B-4EF8-8790-7DFB2908797F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F549312-474D-4933-A727-B6620EA073FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="192">
   <si>
     <t>Proposto</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Alex Buarque</t>
   </si>
   <si>
-    <t>Projeto: Orion Conect | Gerenciamento e fiscalização do transporte público</t>
-  </si>
-  <si>
     <r>
       <t>Autor</t>
     </r>
@@ -272,31 +269,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Sessão home com </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Exo 2"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">carousel </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Exo 2"/>
-        <family val="3"/>
-      </rPr>
-      <t>de imagens que demonstram a essência da empresa</t>
-    </r>
-  </si>
-  <si>
-    <t>Sessão com fundo em imagem embassada e um breve testo de qual é a proposta da empresa</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Sessão onde é listado a visão, missão e valores, cada uma dentro de um componente </t>
     </r>
     <r>
@@ -617,9 +589,6 @@
   </si>
   <si>
     <t>IoT</t>
-  </si>
-  <si>
-    <t>Equipamento arduido para cada ponto de fiscalização de linhas nos terminais</t>
   </si>
   <si>
     <t>Módulo Rfid (RC522) para transportar os dados da viagem</t>
@@ -663,9 +632,6 @@
   </si>
   <si>
     <t>Banco de dados</t>
-  </si>
-  <si>
-    <t>Banco de dados hospoedado na nuvem AZURE</t>
   </si>
   <si>
     <t>Regra de negócio feita em procedures</t>
@@ -733,12 +699,115 @@
   <si>
     <t>Criação dos requisitos</t>
   </si>
+  <si>
+    <t>Sessão com fundo em imagem embassada e um breve texto de qual é a proposta da empresa</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sessão home com </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Exo 2"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">caroussel </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Exo 2"/>
+        <family val="3"/>
+      </rPr>
+      <t>de imagens que demonstram a essência da empresa</t>
+    </r>
+  </si>
+  <si>
+    <t>Banco de dados hospodado na nuvem AZURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">João Pedro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lais </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O banco de dados deve ser em nuvem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação de conta que hospedará o banco </t>
+  </si>
+  <si>
+    <t>Biblioteca JavaScrip</t>
+  </si>
+  <si>
+    <t>A regra de negócio deve ser aplicada de acordo com o escopo do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex Gusmão </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernanda </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os dados devem ser coletados e enviados instanteamente ao banco </t>
+  </si>
+  <si>
+    <t>Banco de dados configurado com tabelas implementadas</t>
+  </si>
+  <si>
+    <t>Vitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O componente deve ser configurado para emitir  dados </t>
+  </si>
+  <si>
+    <t>Configuração do equipamento</t>
+  </si>
+  <si>
+    <t>Sinal de Wi-fii disponível</t>
+  </si>
+  <si>
+    <t>Usuário</t>
+  </si>
+  <si>
+    <t>Respeitar a premissa que indica a necessidade de acesso a internet</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Equipamento arduino para cada ponto de fiscalização de linhas nos terminais</t>
+  </si>
+  <si>
+    <t>Equipamento deve transferir dados</t>
+  </si>
+  <si>
+    <t>Raissa</t>
+  </si>
+  <si>
+    <t>É premissa para o funcionamento do produto que seja implementado,equipamento ao ponto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premissa para funcionamento do produto </t>
+  </si>
+  <si>
+    <t>Destino de veículos</t>
+  </si>
+  <si>
+    <t>Projeto: Zênite | Automação e gerenciamento do transporte urbano</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -887,6 +956,12 @@
       <i/>
       <sz val="10"/>
       <name val="Exo 2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1266,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1487,6 +1562,10 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2461,11 +2540,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:V78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2482,7 +2561,7 @@
     <col min="10" max="10" width="22.42578125" style="50" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" style="50" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" style="50" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" style="50" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" style="7" customWidth="1"/>
     <col min="15" max="15" width="30.5703125" style="50" customWidth="1"/>
     <col min="16" max="16" width="16" style="50" customWidth="1"/>
@@ -2529,7 +2608,7 @@
       <c r="M2" s="68"/>
       <c r="N2" s="69"/>
       <c r="O2" s="73" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="P2" s="73"/>
       <c r="Q2" s="7"/>
@@ -2559,7 +2638,7 @@
     </row>
     <row r="4" spans="2:22" ht="12.75" customHeight="1" thickBot="1">
       <c r="E4" s="58" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
@@ -2571,7 +2650,7 @@
       <c r="M4" s="59"/>
       <c r="N4" s="60"/>
       <c r="O4" s="76" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="76"/>
       <c r="Q4" s="12"/>
@@ -2687,7 +2766,7 @@
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="36"/>
@@ -2698,10 +2777,10 @@
         <v>31</v>
       </c>
       <c r="I8" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
@@ -2715,13 +2794,13 @@
         <v>43890</v>
       </c>
       <c r="R8" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S8" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T8" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U8" s="36" t="s">
         <v>0</v>
@@ -2730,10 +2809,10 @@
     <row r="9" spans="2:22" s="39" customFormat="1" ht="40.5">
       <c r="B9" s="40"/>
       <c r="C9" s="41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="36">
@@ -2746,10 +2825,10 @@
         <v>31</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
@@ -2763,13 +2842,13 @@
         <v>43890</v>
       </c>
       <c r="R9" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S9" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T9" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U9" s="36" t="s">
         <v>0</v>
@@ -2778,10 +2857,10 @@
     <row r="10" spans="2:22" s="39" customFormat="1" ht="40.5">
       <c r="B10" s="40"/>
       <c r="C10" s="41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="36">
@@ -2794,10 +2873,10 @@
         <v>31</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
@@ -2811,13 +2890,13 @@
         <v>43890</v>
       </c>
       <c r="R10" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S10" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T10" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U10" s="36" t="s">
         <v>0</v>
@@ -2826,10 +2905,10 @@
     <row r="11" spans="2:22" s="39" customFormat="1" ht="40.5">
       <c r="B11" s="40"/>
       <c r="C11" s="41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="36">
@@ -2842,10 +2921,10 @@
         <v>31</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
@@ -2859,13 +2938,13 @@
         <v>43890</v>
       </c>
       <c r="R11" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S11" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T11" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U11" s="36" t="s">
         <v>0</v>
@@ -2874,10 +2953,10 @@
     <row r="12" spans="2:22" s="39" customFormat="1" ht="38.25">
       <c r="B12" s="40"/>
       <c r="C12" s="41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E12" s="52"/>
       <c r="F12" s="53">
@@ -2890,10 +2969,10 @@
         <v>31</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K12" s="53"/>
       <c r="L12" s="53"/>
@@ -2907,13 +2986,13 @@
         <v>43890</v>
       </c>
       <c r="R12" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S12" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T12" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U12" s="53" t="s">
         <v>0</v>
@@ -2922,10 +3001,10 @@
     <row r="13" spans="2:22" s="39" customFormat="1" ht="38.25">
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" s="52"/>
       <c r="F13" s="53">
@@ -2938,10 +3017,10 @@
         <v>31</v>
       </c>
       <c r="I13" s="54" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K13" s="53"/>
       <c r="L13" s="53"/>
@@ -2955,13 +3034,13 @@
         <v>43890</v>
       </c>
       <c r="R13" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S13" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T13" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U13" s="53" t="s">
         <v>0</v>
@@ -2970,10 +3049,10 @@
     <row r="14" spans="2:22" s="39" customFormat="1" ht="38.25">
       <c r="B14" s="40"/>
       <c r="C14" s="41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="53">
@@ -2986,10 +3065,10 @@
         <v>31</v>
       </c>
       <c r="I14" s="54" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K14" s="53"/>
       <c r="L14" s="53"/>
@@ -3003,13 +3082,13 @@
         <v>43890</v>
       </c>
       <c r="R14" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S14" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T14" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U14" s="53" t="s">
         <v>0</v>
@@ -3018,10 +3097,10 @@
     <row r="15" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="36">
@@ -3034,10 +3113,10 @@
         <v>30</v>
       </c>
       <c r="I15" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J15" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
@@ -3051,13 +3130,13 @@
         <v>43890</v>
       </c>
       <c r="R15" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S15" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T15" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U15" s="36" t="s">
         <v>0</v>
@@ -3069,7 +3148,7 @@
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="36">
@@ -3082,10 +3161,10 @@
         <v>31</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K16" s="36"/>
       <c r="L16" s="36"/>
@@ -3099,23 +3178,25 @@
         <v>43890</v>
       </c>
       <c r="R16" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S16" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T16" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="U16" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="U16" s="36" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B17" s="40"/>
       <c r="C17" s="41" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="36">
@@ -3128,10 +3209,10 @@
         <v>31</v>
       </c>
       <c r="I17" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="J17" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J17" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
@@ -3145,23 +3226,25 @@
         <v>43890</v>
       </c>
       <c r="R17" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S17" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T17" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="U17" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="U17" s="36" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B18" s="40"/>
       <c r="C18" s="41" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="36">
@@ -3174,10 +3257,10 @@
         <v>31</v>
       </c>
       <c r="I18" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="J18" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J18" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
@@ -3191,23 +3274,25 @@
         <v>43890</v>
       </c>
       <c r="R18" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S18" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T18" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="U18" s="36"/>
-    </row>
-    <row r="19" spans="2:21" s="39" customFormat="1" ht="40.5">
+        <v>162</v>
+      </c>
+      <c r="U18" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B19" s="40"/>
       <c r="C19" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="36">
@@ -3220,16 +3305,16 @@
         <v>30</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J19" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
-      <c r="N19" s="35" t="s">
-        <v>61</v>
+      <c r="N19" s="51" t="s">
+        <v>51</v>
       </c>
       <c r="O19" s="34"/>
       <c r="P19" s="37">
@@ -3239,13 +3324,13 @@
         <v>43890</v>
       </c>
       <c r="R19" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S19" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T19" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U19" s="36" t="s">
         <v>0</v>
@@ -3254,10 +3339,10 @@
     <row r="20" spans="2:21" s="39" customFormat="1" ht="67.5">
       <c r="B20" s="40"/>
       <c r="C20" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="36">
@@ -3270,16 +3355,16 @@
         <v>31</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
       <c r="M20" s="36"/>
-      <c r="N20" s="35" t="s">
-        <v>61</v>
+      <c r="N20" s="51" t="s">
+        <v>51</v>
       </c>
       <c r="O20" s="34"/>
       <c r="P20" s="37">
@@ -3289,13 +3374,13 @@
         <v>43890</v>
       </c>
       <c r="R20" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S20" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T20" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U20" s="36" t="s">
         <v>0</v>
@@ -3304,10 +3389,10 @@
     <row r="21" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B21" s="40"/>
       <c r="C21" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="36">
@@ -3320,10 +3405,10 @@
         <v>31</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K21" s="36"/>
       <c r="L21" s="36"/>
@@ -3337,13 +3422,13 @@
         <v>43890</v>
       </c>
       <c r="R21" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S21" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T21" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U21" s="36" t="s">
         <v>0</v>
@@ -3352,10 +3437,10 @@
     <row r="22" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B22" s="40"/>
       <c r="C22" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="36"/>
@@ -3366,10 +3451,10 @@
         <v>31</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K22" s="36"/>
       <c r="L22" s="36"/>
@@ -3383,13 +3468,13 @@
         <v>43890</v>
       </c>
       <c r="R22" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S22" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T22" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U22" s="36" t="s">
         <v>0</v>
@@ -3398,10 +3483,10 @@
     <row r="23" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B23" s="40"/>
       <c r="C23" s="41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E23" s="35"/>
       <c r="F23" s="36">
@@ -3414,10 +3499,10 @@
         <v>30</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K23" s="36"/>
       <c r="L23" s="36"/>
@@ -3431,13 +3516,13 @@
         <v>43890</v>
       </c>
       <c r="R23" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S23" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T23" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U23" s="36" t="s">
         <v>0</v>
@@ -3446,10 +3531,10 @@
     <row r="24" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B24" s="40"/>
       <c r="C24" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E24" s="35"/>
       <c r="F24" s="36">
@@ -3462,10 +3547,10 @@
         <v>30</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K24" s="36"/>
       <c r="L24" s="36"/>
@@ -3479,13 +3564,13 @@
         <v>43890</v>
       </c>
       <c r="R24" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S24" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T24" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U24" s="36" t="s">
         <v>0</v>
@@ -3494,10 +3579,10 @@
     <row r="25" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B25" s="40"/>
       <c r="C25" s="41" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E25" s="35"/>
       <c r="F25" s="36">
@@ -3510,10 +3595,10 @@
         <v>30</v>
       </c>
       <c r="I25" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K25" s="36"/>
       <c r="L25" s="36"/>
@@ -3527,13 +3612,13 @@
         <v>43890</v>
       </c>
       <c r="R25" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S25" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T25" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U25" s="36" t="s">
         <v>0</v>
@@ -3542,10 +3627,10 @@
     <row r="26" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B26" s="40"/>
       <c r="C26" s="41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="36">
@@ -3558,10 +3643,10 @@
         <v>30</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J26" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K26" s="36"/>
       <c r="L26" s="36"/>
@@ -3575,13 +3660,13 @@
         <v>43890</v>
       </c>
       <c r="R26" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S26" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T26" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U26" s="36" t="s">
         <v>0</v>
@@ -3590,10 +3675,10 @@
     <row r="27" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B27" s="40"/>
       <c r="C27" s="41" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E27" s="35"/>
       <c r="F27" s="36">
@@ -3606,10 +3691,10 @@
         <v>30</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J27" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K27" s="36"/>
       <c r="L27" s="36"/>
@@ -3623,13 +3708,13 @@
         <v>43890</v>
       </c>
       <c r="R27" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S27" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T27" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U27" s="36" t="s">
         <v>0</v>
@@ -3638,10 +3723,10 @@
     <row r="28" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B28" s="40"/>
       <c r="C28" s="41" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E28" s="35"/>
       <c r="F28" s="36">
@@ -3654,16 +3739,16 @@
         <v>30</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J28" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K28" s="36"/>
       <c r="L28" s="36"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="35" t="s">
-        <v>76</v>
+      <c r="N28" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="O28" s="34"/>
       <c r="P28" s="37">
@@ -3673,25 +3758,25 @@
         <v>43890</v>
       </c>
       <c r="R28" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S28" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T28" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U28" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="29" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B29" s="40"/>
       <c r="C29" s="41" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="36">
@@ -3704,16 +3789,16 @@
         <v>30</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J29" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K29" s="36"/>
       <c r="L29" s="36"/>
       <c r="M29" s="36"/>
-      <c r="N29" s="35" t="s">
-        <v>78</v>
+      <c r="N29" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="O29" s="34"/>
       <c r="P29" s="37">
@@ -3723,25 +3808,25 @@
         <v>43890</v>
       </c>
       <c r="R29" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S29" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T29" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U29" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="30" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B30" s="40"/>
       <c r="C30" s="41" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E30" s="35"/>
       <c r="F30" s="36">
@@ -3754,16 +3839,16 @@
         <v>30</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K30" s="36"/>
       <c r="L30" s="36"/>
       <c r="M30" s="36"/>
-      <c r="N30" s="35" t="s">
-        <v>77</v>
+      <c r="N30" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="O30" s="34"/>
       <c r="P30" s="37">
@@ -3773,25 +3858,25 @@
         <v>43890</v>
       </c>
       <c r="R30" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S30" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T30" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U30" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="31" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B31" s="40"/>
       <c r="C31" s="41" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="36">
@@ -3804,16 +3889,16 @@
         <v>30</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J31" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K31" s="36"/>
       <c r="L31" s="36"/>
       <c r="M31" s="36"/>
-      <c r="N31" s="35" t="s">
-        <v>79</v>
+      <c r="N31" s="34" t="s">
+        <v>67</v>
       </c>
       <c r="O31" s="34"/>
       <c r="P31" s="37">
@@ -3823,13 +3908,13 @@
         <v>43890</v>
       </c>
       <c r="R31" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S31" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T31" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U31" s="36" t="s">
         <v>0</v>
@@ -3838,10 +3923,10 @@
     <row r="32" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B32" s="40"/>
       <c r="C32" s="41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E32" s="35"/>
       <c r="F32" s="36">
@@ -3854,10 +3939,10 @@
         <v>31</v>
       </c>
       <c r="I32" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J32" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K32" s="36"/>
       <c r="L32" s="36"/>
@@ -3871,13 +3956,13 @@
         <v>43890</v>
       </c>
       <c r="R32" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S32" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T32" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U32" s="36" t="s">
         <v>0</v>
@@ -3886,10 +3971,10 @@
     <row r="33" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B33" s="40"/>
       <c r="C33" s="41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E33" s="35"/>
       <c r="F33" s="36">
@@ -3902,10 +3987,10 @@
         <v>31</v>
       </c>
       <c r="I33" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J33" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J33" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K33" s="36"/>
       <c r="L33" s="36"/>
@@ -3919,13 +4004,13 @@
         <v>43890</v>
       </c>
       <c r="R33" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S33" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T33" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U33" s="36" t="s">
         <v>0</v>
@@ -3934,10 +4019,10 @@
     <row r="34" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B34" s="40"/>
       <c r="C34" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="36">
@@ -3950,10 +4035,10 @@
         <v>30</v>
       </c>
       <c r="I34" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J34" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K34" s="36"/>
       <c r="L34" s="36"/>
@@ -3967,25 +4052,25 @@
         <v>43890</v>
       </c>
       <c r="R34" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S34" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T34" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U34" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="35" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B35" s="40"/>
       <c r="C35" s="41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E35" s="35"/>
       <c r="F35" s="36">
@@ -3998,16 +4083,16 @@
         <v>30</v>
       </c>
       <c r="I35" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J35" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J35" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K35" s="36"/>
       <c r="L35" s="36"/>
       <c r="M35" s="36"/>
-      <c r="N35" s="35" t="s">
-        <v>117</v>
+      <c r="N35" s="34" t="s">
+        <v>157</v>
       </c>
       <c r="O35" s="34"/>
       <c r="P35" s="37">
@@ -4017,13 +4102,13 @@
         <v>43890</v>
       </c>
       <c r="R35" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S35" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T35" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U35" s="36" t="s">
         <v>0</v>
@@ -4032,10 +4117,10 @@
     <row r="36" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B36" s="40"/>
       <c r="C36" s="41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E36" s="35"/>
       <c r="F36" s="36">
@@ -4048,10 +4133,10 @@
         <v>31</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J36" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K36" s="36"/>
       <c r="L36" s="36"/>
@@ -4065,13 +4150,13 @@
         <v>43890</v>
       </c>
       <c r="R36" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S36" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T36" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U36" s="36" t="s">
         <v>0</v>
@@ -4080,10 +4165,10 @@
     <row r="37" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B37" s="40"/>
       <c r="C37" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E37" s="35"/>
       <c r="F37" s="36">
@@ -4096,15 +4181,17 @@
         <v>31</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J37" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
       <c r="M37" s="36"/>
-      <c r="N37" s="35"/>
+      <c r="N37" s="81" t="s">
+        <v>171</v>
+      </c>
       <c r="O37" s="34"/>
       <c r="P37" s="37">
         <v>43890</v>
@@ -4113,13 +4200,13 @@
         <v>43890</v>
       </c>
       <c r="R37" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S37" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T37" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U37" s="36" t="s">
         <v>0</v>
@@ -4128,10 +4215,10 @@
     <row r="38" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B38" s="40"/>
       <c r="C38" s="41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E38" s="35"/>
       <c r="F38" s="36">
@@ -4144,16 +4231,16 @@
         <v>30</v>
       </c>
       <c r="I38" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J38" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K38" s="36"/>
       <c r="L38" s="36"/>
       <c r="M38" s="36"/>
-      <c r="N38" s="35" t="s">
-        <v>120</v>
+      <c r="N38" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O38" s="34"/>
       <c r="P38" s="37">
@@ -4163,13 +4250,13 @@
         <v>43890</v>
       </c>
       <c r="R38" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S38" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T38" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U38" s="36" t="s">
         <v>0</v>
@@ -4178,10 +4265,10 @@
     <row r="39" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B39" s="40"/>
       <c r="C39" s="41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E39" s="35"/>
       <c r="F39" s="36">
@@ -4194,16 +4281,16 @@
         <v>30</v>
       </c>
       <c r="I39" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J39" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K39" s="36"/>
       <c r="L39" s="36"/>
       <c r="M39" s="36"/>
-      <c r="N39" s="35" t="s">
-        <v>120</v>
+      <c r="N39" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O39" s="34"/>
       <c r="P39" s="37">
@@ -4213,13 +4300,13 @@
         <v>43890</v>
       </c>
       <c r="R39" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S39" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T39" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U39" s="36" t="s">
         <v>0</v>
@@ -4228,10 +4315,10 @@
     <row r="40" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B40" s="40"/>
       <c r="C40" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D40" s="34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E40" s="35"/>
       <c r="F40" s="36">
@@ -4244,16 +4331,16 @@
         <v>30</v>
       </c>
       <c r="I40" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J40" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K40" s="36"/>
       <c r="L40" s="36"/>
       <c r="M40" s="36"/>
-      <c r="N40" s="35" t="s">
-        <v>120</v>
+      <c r="N40" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O40" s="34"/>
       <c r="P40" s="37">
@@ -4263,25 +4350,25 @@
         <v>43890</v>
       </c>
       <c r="R40" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S40" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T40" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U40" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="41" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B41" s="40"/>
       <c r="C41" s="41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E41" s="35"/>
       <c r="F41" s="36">
@@ -4294,16 +4381,16 @@
         <v>30</v>
       </c>
       <c r="I41" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J41" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K41" s="36"/>
       <c r="L41" s="36"/>
       <c r="M41" s="36"/>
-      <c r="N41" s="35" t="s">
-        <v>120</v>
+      <c r="N41" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O41" s="34"/>
       <c r="P41" s="37">
@@ -4313,13 +4400,13 @@
         <v>43890</v>
       </c>
       <c r="R41" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S41" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T41" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U41" s="36" t="s">
         <v>0</v>
@@ -4328,10 +4415,10 @@
     <row r="42" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B42" s="40"/>
       <c r="C42" s="41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D42" s="34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E42" s="35"/>
       <c r="F42" s="36">
@@ -4344,16 +4431,16 @@
         <v>30</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J42" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K42" s="36"/>
       <c r="L42" s="36"/>
       <c r="M42" s="36"/>
-      <c r="N42" s="35" t="s">
-        <v>120</v>
+      <c r="N42" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O42" s="34"/>
       <c r="P42" s="37">
@@ -4363,13 +4450,13 @@
         <v>43890</v>
       </c>
       <c r="R42" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S42" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T42" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U42" s="36" t="s">
         <v>0</v>
@@ -4378,10 +4465,10 @@
     <row r="43" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B43" s="40"/>
       <c r="C43" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E43" s="35"/>
       <c r="F43" s="36">
@@ -4394,16 +4481,16 @@
         <v>30</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J43" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K43" s="36"/>
       <c r="L43" s="36"/>
       <c r="M43" s="36"/>
-      <c r="N43" s="35" t="s">
-        <v>120</v>
+      <c r="N43" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O43" s="34"/>
       <c r="P43" s="37">
@@ -4413,25 +4500,25 @@
         <v>43890</v>
       </c>
       <c r="R43" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S43" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T43" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U43" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="44" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B44" s="40"/>
       <c r="C44" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E44" s="35"/>
       <c r="F44" s="36">
@@ -4444,16 +4531,16 @@
         <v>30</v>
       </c>
       <c r="I44" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J44" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K44" s="36"/>
       <c r="L44" s="36"/>
       <c r="M44" s="36"/>
-      <c r="N44" s="35" t="s">
-        <v>120</v>
+      <c r="N44" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O44" s="34"/>
       <c r="P44" s="37">
@@ -4463,13 +4550,13 @@
         <v>43890</v>
       </c>
       <c r="R44" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S44" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T44" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U44" s="36" t="s">
         <v>0</v>
@@ -4478,10 +4565,10 @@
     <row r="45" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B45" s="40"/>
       <c r="C45" s="41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E45" s="35"/>
       <c r="F45" s="36">
@@ -4494,16 +4581,16 @@
         <v>30</v>
       </c>
       <c r="I45" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J45" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K45" s="36"/>
       <c r="L45" s="36"/>
       <c r="M45" s="36"/>
-      <c r="N45" s="35" t="s">
-        <v>120</v>
+      <c r="N45" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O45" s="34"/>
       <c r="P45" s="37">
@@ -4513,13 +4600,13 @@
         <v>43890</v>
       </c>
       <c r="R45" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S45" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T45" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U45" s="36" t="s">
         <v>0</v>
@@ -4528,10 +4615,10 @@
     <row r="46" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B46" s="40"/>
       <c r="C46" s="41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E46" s="35"/>
       <c r="F46" s="36">
@@ -4544,16 +4631,16 @@
         <v>30</v>
       </c>
       <c r="I46" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J46" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
       <c r="M46" s="36"/>
-      <c r="N46" s="35" t="s">
-        <v>120</v>
+      <c r="N46" s="34" t="s">
+        <v>88</v>
       </c>
       <c r="O46" s="34"/>
       <c r="P46" s="37">
@@ -4563,13 +4650,13 @@
         <v>43890</v>
       </c>
       <c r="R46" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S46" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T46" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U46" s="36" t="s">
         <v>0</v>
@@ -4578,10 +4665,10 @@
     <row r="47" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B47" s="40"/>
       <c r="C47" s="41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E47" s="35"/>
       <c r="F47" s="36">
@@ -4594,10 +4681,10 @@
         <v>30</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J47" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K47" s="36"/>
       <c r="L47" s="36"/>
@@ -4611,13 +4698,13 @@
         <v>43890</v>
       </c>
       <c r="R47" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S47" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T47" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U47" s="36" t="s">
         <v>0</v>
@@ -4626,10 +4713,10 @@
     <row r="48" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B48" s="40"/>
       <c r="C48" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E48" s="35"/>
       <c r="F48" s="36">
@@ -4642,10 +4729,10 @@
         <v>30</v>
       </c>
       <c r="I48" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J48" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
@@ -4659,13 +4746,13 @@
         <v>43890</v>
       </c>
       <c r="R48" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S48" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T48" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U48" s="36" t="s">
         <v>0</v>
@@ -4674,10 +4761,10 @@
     <row r="49" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B49" s="40"/>
       <c r="C49" s="41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E49" s="35"/>
       <c r="F49" s="36">
@@ -4690,10 +4777,10 @@
         <v>31</v>
       </c>
       <c r="I49" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J49" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J49" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K49" s="36"/>
       <c r="L49" s="36"/>
@@ -4707,13 +4794,13 @@
         <v>43890</v>
       </c>
       <c r="R49" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S49" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T49" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U49" s="36" t="s">
         <v>0</v>
@@ -4722,10 +4809,10 @@
     <row r="50" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B50" s="40"/>
       <c r="C50" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E50" s="35"/>
       <c r="F50" s="36">
@@ -4738,10 +4825,10 @@
         <v>30</v>
       </c>
       <c r="I50" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J50" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J50" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K50" s="36"/>
       <c r="L50" s="36"/>
@@ -4755,13 +4842,13 @@
         <v>43890</v>
       </c>
       <c r="R50" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S50" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T50" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U50" s="36" t="s">
         <v>0</v>
@@ -4770,10 +4857,10 @@
     <row r="51" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B51" s="40"/>
       <c r="C51" s="41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E51" s="35"/>
       <c r="F51" s="36">
@@ -4786,10 +4873,10 @@
         <v>30</v>
       </c>
       <c r="I51" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J51" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J51" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K51" s="36"/>
       <c r="L51" s="36"/>
@@ -4803,13 +4890,13 @@
         <v>43890</v>
       </c>
       <c r="R51" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S51" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T51" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U51" s="36" t="s">
         <v>0</v>
@@ -4818,10 +4905,10 @@
     <row r="52" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B52" s="40"/>
       <c r="C52" s="41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E52" s="35"/>
       <c r="F52" s="36">
@@ -4834,10 +4921,10 @@
         <v>30</v>
       </c>
       <c r="I52" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J52" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J52" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K52" s="36"/>
       <c r="L52" s="36"/>
@@ -4851,13 +4938,13 @@
         <v>43890</v>
       </c>
       <c r="R52" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S52" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T52" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U52" s="36" t="s">
         <v>0</v>
@@ -4866,10 +4953,10 @@
     <row r="53" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B53" s="40"/>
       <c r="C53" s="41" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E53" s="35"/>
       <c r="F53" s="36">
@@ -4882,10 +4969,10 @@
         <v>30</v>
       </c>
       <c r="I53" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J53" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J53" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K53" s="36"/>
       <c r="L53" s="36"/>
@@ -4899,13 +4986,13 @@
         <v>43890</v>
       </c>
       <c r="R53" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S53" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T53" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U53" s="36" t="s">
         <v>0</v>
@@ -4914,10 +5001,10 @@
     <row r="54" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B54" s="40"/>
       <c r="C54" s="41" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E54" s="35"/>
       <c r="F54" s="36">
@@ -4930,10 +5017,10 @@
         <v>30</v>
       </c>
       <c r="I54" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J54" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J54" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K54" s="36"/>
       <c r="L54" s="36"/>
@@ -4947,13 +5034,13 @@
         <v>43890</v>
       </c>
       <c r="R54" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S54" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T54" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U54" s="36" t="s">
         <v>0</v>
@@ -4962,10 +5049,10 @@
     <row r="55" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B55" s="40"/>
       <c r="C55" s="41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E55" s="35"/>
       <c r="F55" s="36">
@@ -4978,10 +5065,10 @@
         <v>30</v>
       </c>
       <c r="I55" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J55" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K55" s="36"/>
       <c r="L55" s="36"/>
@@ -4995,13 +5082,13 @@
         <v>43890</v>
       </c>
       <c r="R55" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S55" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T55" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U55" s="36" t="s">
         <v>0</v>
@@ -5010,10 +5097,10 @@
     <row r="56" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B56" s="40"/>
       <c r="C56" s="41" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E56" s="35"/>
       <c r="F56" s="36">
@@ -5026,10 +5113,10 @@
         <v>30</v>
       </c>
       <c r="I56" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J56" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K56" s="36"/>
       <c r="L56" s="36"/>
@@ -5043,13 +5130,13 @@
         <v>43890</v>
       </c>
       <c r="R56" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S56" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T56" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U56" s="36" t="s">
         <v>0</v>
@@ -5058,10 +5145,10 @@
     <row r="57" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B57" s="40"/>
       <c r="C57" s="41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E57" s="35"/>
       <c r="F57" s="36">
@@ -5074,32 +5161,32 @@
         <v>30</v>
       </c>
       <c r="I57" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J57" s="36" t="s">
         <v>155</v>
-      </c>
-      <c r="J57" s="36" t="s">
-        <v>160</v>
       </c>
       <c r="K57" s="36"/>
       <c r="L57" s="36"/>
       <c r="M57" s="36"/>
       <c r="N57" s="35"/>
       <c r="O57" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="P57" s="37">
+        <v>43890</v>
+      </c>
+      <c r="Q57" s="37">
+        <v>43890</v>
+      </c>
+      <c r="R57" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="S57" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="P57" s="37">
-        <v>43890</v>
-      </c>
-      <c r="Q57" s="37">
-        <v>43890</v>
-      </c>
-      <c r="R57" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="S57" s="36" t="s">
-        <v>168</v>
-      </c>
       <c r="T57" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U57" s="36" t="s">
         <v>0</v>
@@ -5108,10 +5195,10 @@
     <row r="58" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B58" s="40"/>
       <c r="C58" s="41" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E58" s="35"/>
       <c r="F58" s="36">
@@ -5124,10 +5211,10 @@
         <v>30</v>
       </c>
       <c r="I58" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J58" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K58" s="36"/>
       <c r="L58" s="36"/>
@@ -5141,13 +5228,13 @@
         <v>43890</v>
       </c>
       <c r="R58" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S58" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T58" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U58" s="36" t="s">
         <v>0</v>
@@ -5159,7 +5246,7 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E59" s="35"/>
       <c r="F59" s="36">
@@ -5172,10 +5259,10 @@
         <v>31</v>
       </c>
       <c r="I59" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J59" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K59" s="36"/>
       <c r="L59" s="36"/>
@@ -5189,25 +5276,25 @@
         <v>43890</v>
       </c>
       <c r="R59" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S59" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T59" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U59" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="60" spans="2:21" s="39" customFormat="1" ht="67.5">
       <c r="B60" s="40"/>
       <c r="C60" s="41" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="E60" s="35"/>
       <c r="F60" s="36">
@@ -5220,16 +5307,26 @@
         <v>31</v>
       </c>
       <c r="I60" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J60" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K60" s="36"/>
-      <c r="L60" s="36"/>
-      <c r="M60" s="36"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="34"/>
+        <v>155</v>
+      </c>
+      <c r="K60" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="L60" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="M60" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="N60" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="O60" s="34" t="s">
+        <v>190</v>
+      </c>
       <c r="P60" s="37">
         <v>43890</v>
       </c>
@@ -5237,25 +5334,25 @@
         <v>43890</v>
       </c>
       <c r="R60" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S60" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T60" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U60" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="61" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B61" s="40"/>
       <c r="C61" s="41" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D61" s="34" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E61" s="35"/>
       <c r="F61" s="36">
@@ -5268,18 +5365,26 @@
         <v>31</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J61" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K61" s="36"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="36"/>
-      <c r="N61" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="O61" s="34"/>
+        <v>155</v>
+      </c>
+      <c r="K61" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="L61" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M61" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="N61" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="O61" s="34" t="s">
+        <v>185</v>
+      </c>
       <c r="P61" s="37">
         <v>43890</v>
       </c>
@@ -5287,25 +5392,25 @@
         <v>43890</v>
       </c>
       <c r="R61" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S61" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T61" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U61" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="62" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B62" s="40"/>
       <c r="C62" s="41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E62" s="35"/>
       <c r="F62" s="36">
@@ -5318,17 +5423,25 @@
         <v>31</v>
       </c>
       <c r="I62" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J62" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K62" s="36"/>
-      <c r="L62" s="36"/>
-      <c r="M62" s="36"/>
-      <c r="N62" s="35"/>
+        <v>155</v>
+      </c>
+      <c r="K62" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="L62" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="M62" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="N62" s="35" t="s">
+        <v>181</v>
+      </c>
       <c r="O62" s="34" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="P62" s="37">
         <v>43890</v>
@@ -5337,25 +5450,25 @@
         <v>43890</v>
       </c>
       <c r="R62" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S62" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T62" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U62" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="63" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B63" s="40"/>
       <c r="C63" s="41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E63" s="35"/>
       <c r="F63" s="36">
@@ -5368,18 +5481,26 @@
         <v>31</v>
       </c>
       <c r="I63" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J63" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K63" s="36"/>
-      <c r="L63" s="36"/>
-      <c r="M63" s="36"/>
-      <c r="N63" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="O63" s="34"/>
+        <v>155</v>
+      </c>
+      <c r="K63" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="L63" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M63" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="N63" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="O63" s="34" t="s">
+        <v>185</v>
+      </c>
       <c r="P63" s="37">
         <v>43890</v>
       </c>
@@ -5387,25 +5508,25 @@
         <v>43890</v>
       </c>
       <c r="R63" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S63" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T63" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U63" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="64" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B64" s="40"/>
       <c r="C64" s="41" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E64" s="35"/>
       <c r="F64" s="36">
@@ -5418,18 +5539,26 @@
         <v>31</v>
       </c>
       <c r="I64" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J64" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K64" s="36"/>
-      <c r="L64" s="36"/>
-      <c r="M64" s="36"/>
-      <c r="N64" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="O64" s="34"/>
+        <v>155</v>
+      </c>
+      <c r="K64" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="L64" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="M64" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="N64" s="82" t="s">
+        <v>180</v>
+      </c>
+      <c r="O64" s="34" t="s">
+        <v>185</v>
+      </c>
       <c r="P64" s="37">
         <v>43890</v>
       </c>
@@ -5437,25 +5566,25 @@
         <v>43890</v>
       </c>
       <c r="R64" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S64" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T64" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U64" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="65" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B65" s="40"/>
       <c r="C65" s="41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D65" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E65" s="35"/>
       <c r="F65" s="36">
@@ -5468,17 +5597,25 @@
         <v>30</v>
       </c>
       <c r="I65" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J65" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K65" s="36"/>
-      <c r="L65" s="36"/>
-      <c r="M65" s="36"/>
-      <c r="N65" s="35"/>
+        <v>155</v>
+      </c>
+      <c r="K65" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="L65" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="M65" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="N65" s="35" t="s">
+        <v>177</v>
+      </c>
       <c r="O65" s="34" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="P65" s="37">
         <v>43890</v>
@@ -5487,13 +5624,13 @@
         <v>43890</v>
       </c>
       <c r="R65" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S65" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T65" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U65" s="36" t="s">
         <v>0</v>
@@ -5505,7 +5642,7 @@
       </c>
       <c r="C66" s="41"/>
       <c r="D66" s="34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E66" s="35"/>
       <c r="F66" s="36">
@@ -5518,16 +5655,20 @@
         <v>31</v>
       </c>
       <c r="I66" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J66" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K66" s="36"/>
       <c r="L66" s="36"/>
       <c r="M66" s="36"/>
-      <c r="N66" s="35"/>
-      <c r="O66" s="34"/>
+      <c r="N66" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="O66" s="34" t="s">
+        <v>175</v>
+      </c>
       <c r="P66" s="37">
         <v>43890</v>
       </c>
@@ -5535,25 +5676,25 @@
         <v>43890</v>
       </c>
       <c r="R66" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S66" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T66" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U66" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="67" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B67" s="40"/>
       <c r="C67" s="41" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="E67" s="35"/>
       <c r="F67" s="36">
@@ -5566,18 +5707,26 @@
         <v>31</v>
       </c>
       <c r="I67" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J67" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="K67" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="L67" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="M67" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="N67" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="O67" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="K67" s="36"/>
-      <c r="L67" s="36"/>
-      <c r="M67" s="36"/>
-      <c r="N67" s="35"/>
-      <c r="O67" s="34" t="s">
-        <v>165</v>
-      </c>
       <c r="P67" s="37">
         <v>43890</v>
       </c>
@@ -5585,25 +5734,25 @@
         <v>43890</v>
       </c>
       <c r="R67" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S67" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T67" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U67" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="68" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B68" s="40"/>
       <c r="C68" s="41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E68" s="35"/>
       <c r="F68" s="36">
@@ -5616,18 +5765,26 @@
         <v>31</v>
       </c>
       <c r="I68" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J68" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="K68" s="36"/>
-      <c r="L68" s="36"/>
-      <c r="M68" s="36"/>
-      <c r="N68" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="O68" s="34"/>
+        <v>155</v>
+      </c>
+      <c r="K68" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="L68" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="M68" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="N68" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="O68" s="34" t="s">
+        <v>175</v>
+      </c>
       <c r="P68" s="37">
         <v>43890</v>
       </c>
@@ -5635,13 +5792,13 @@
         <v>43890</v>
       </c>
       <c r="R68" s="36" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="S68" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="T68" s="38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="U68" s="36" t="s">
         <v>0</v>

</xml_diff>